<commit_message>
ETL ARCCHIVOS EXCEL FIX BUGS
</commit_message>
<xml_diff>
--- a/Proyecto_DMD/Excel/Excel_ordenados/excel_1994.xlsx
+++ b/Proyecto_DMD/Excel/Excel_ordenados/excel_1994.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\Desktop\Proyecto_DMD\Excel\Excel_ordenados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18696" windowHeight="6516"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" r:id="rId1" name="Hoja1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" fullCalcOnLoad="true"/>
+  <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -371,9 +378,9 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row spans="1:5" ht="15.6" outlineLevel="0" r="1">
+    <row spans="1:5" ht="15.6" x14ac:dyDescent="0.3" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>